<commit_message>
Pie and Bar chart 14-09-2025
</commit_message>
<xml_diff>
--- a/Data & Visualization Basics/2.2 Pie Chart & Bar Chart/expenses_and_apple_revenue.xlsx
+++ b/Data & Visualization Basics/2.2 Pie Chart & Bar Chart/expenses_and_apple_revenue.xlsx
@@ -1,47 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ashish\Data Science\Math-and-Statistics-DS\Data &amp; Visualization Basics\2.2 Pie Chart &amp; Bar Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF366DD-A19D-4B77-894A-1944E0A62B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC55EA3-80D2-4E3F-9B42-658F1618F2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{9530BDCB-4E13-4924-AE12-09A760334EFF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{9530BDCB-4E13-4924-AE12-09A760334EFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenses 1" sheetId="8" r:id="rId1"/>
     <sheet name="Expenses 1 Self" sheetId="10" r:id="rId2"/>
     <sheet name="Expenses 2" sheetId="9" r:id="rId3"/>
     <sheet name="Expenses 2 Self" sheetId="11" r:id="rId4"/>
-    <sheet name="Apple's Revenue" sheetId="2" r:id="rId5"/>
-    <sheet name="Apple's Revenue Self" sheetId="12" r:id="rId6"/>
+    <sheet name="Ashish_AA" sheetId="13" r:id="rId5"/>
+    <sheet name="Apple's Revenue" sheetId="2" r:id="rId6"/>
+    <sheet name="Apple's Revenue Self" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
   <si>
     <t>Groceries</t>
   </si>
@@ -639,6 +629,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -646,7 +637,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:gradFill flip="none" rotWithShape="1">
@@ -1165,6 +1155,1166 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Expenses</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-6C98-4089-AD24-B84035D9AADC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-6C98-4089-AD24-B84035D9AADC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-6C98-4089-AD24-B84035D9AADC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-6C98-4089-AD24-B84035D9AADC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-6C98-4089-AD24-B84035D9AADC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-6C98-4089-AD24-B84035D9AADC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-6C98-4089-AD24-B84035D9AADC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-6C98-4089-AD24-B84035D9AADC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-6C98-4089-AD24-B84035D9AADC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-6C98-4089-AD24-B84035D9AADC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="95000"/>
+                      <a:alpha val="54000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Expenses 2 Self'!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Rent</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Restaurants</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Groceries</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Electricity bill</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Phone bill</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fuel cost</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Insurance</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Clothes</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Medicines</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Donations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Expenses 2 Self'!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>450</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C4DB-481B-BCC1-8DAA670ED132}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Expenses 2 Self'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Expenses</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Expenses 2 Self'!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Rent</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Restaurants</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Groceries</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Electricity bill</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Phone bill</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fuel cost</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Insurance</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Clothes</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Medicines</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Donations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Expenses 2 Self'!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>450</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C687-4686-9153-D70F3CC1D4F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="115"/>
+        <c:overlap val="-20"/>
+        <c:axId val="1632608399"/>
+        <c:axId val="1632600719"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1632608399"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1632600719"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1632600719"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1632608399"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Ashish_AA!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Revenue</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1379,228 +2529,6 @@
               </a:effectLst>
             </c:spPr>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent6">
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent6">
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent6">
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="63000"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="60000"/>
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="60000"/>
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="60000"/>
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="63000"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="60000"/>
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="60000"/>
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="60000"/>
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="63000"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent3">
-                      <a:lumMod val="60000"/>
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent3">
-                      <a:lumMod val="60000"/>
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent3">
-                      <a:lumMod val="60000"/>
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="63000"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent4">
-                      <a:lumMod val="60000"/>
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent4">
-                      <a:lumMod val="60000"/>
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent4">
-                      <a:lumMod val="60000"/>
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="63000"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -1632,10 +2560,10 @@
             </c:txPr>
             <c:dLblPos val="bestFit"/>
             <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
+            <c:showVal val="0"/>
             <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:leaderLines>
@@ -1656,92 +2584,62 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>'Expenses 2 Self'!$A$2:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
+            <c:numRef>
+              <c:f>Ashish_AA!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Rent</c:v>
+                  <c:v>2018</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Restaurants</c:v>
+                  <c:v>2019</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Groceries</c:v>
+                  <c:v>2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Electricity bill</c:v>
+                  <c:v>2021</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Phone bill</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Fuel cost</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Insurance</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Clothes</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Medicines</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Donations</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Expenses 2 Self'!$B$2:$B$11</c:f>
+              <c:f>Ashish_AA!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>15000</c:v>
+                  <c:v>265.60000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>260.10000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5100</c:v>
+                  <c:v>274.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3200</c:v>
+                  <c:v>365.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4600</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>450</c:v>
+                  <c:v>385.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C4DB-481B-BCC1-8DAA670ED132}"/>
+              <c16:uniqueId val="{00000000-E0C8-41EF-9941-D29F6A2DFE53}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="bestFit"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1790,13 +2688,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1843,7 +2734,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1897,7 +2788,7 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="bar"/>
+        <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -1905,11 +2796,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Expenses 2 Self'!$B$1</c:f>
+              <c:f>Ashish_AA!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Expenses</c:v>
+                  <c:v>Revenue</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1953,109 +2844,203 @@
             </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
-            <c:strRef>
-              <c:f>'Expenses 2 Self'!$A$2:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
+            <c:numRef>
+              <c:f>Ashish_AA!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Rent</c:v>
+                  <c:v>2018</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Restaurants</c:v>
+                  <c:v>2019</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Groceries</c:v>
+                  <c:v>2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Electricity bill</c:v>
+                  <c:v>2021</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Phone bill</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Fuel cost</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Insurance</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Clothes</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Medicines</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Donations</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Expenses 2 Self'!$B$2:$B$11</c:f>
+              <c:f>Ashish_AA!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>15000</c:v>
+                  <c:v>265.60000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>260.10000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5100</c:v>
+                  <c:v>274.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3200</c:v>
+                  <c:v>365.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4600</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>450</c:v>
+                  <c:v>385.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C687-4686-9153-D70F3CC1D4F5}"/>
+              <c16:uniqueId val="{00000000-D8FD-4854-86EF-81DD21D666DD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="115"/>
-        <c:overlap val="-20"/>
-        <c:axId val="1632608399"/>
-        <c:axId val="1632600719"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="985312575"/>
+        <c:axId val="985298655"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1632608399"/>
+        <c:axId val="985312575"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>YEAR</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2092,7 +3077,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632600719"/>
+        <c:crossAx val="985298655"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2100,12 +3085,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632600719"/>
+        <c:axId val="985298655"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2120,6 +3105,59 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>ReVENUE</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2150,7 +3188,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632608399"/>
+        <c:crossAx val="985312575"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2210,7 +3248,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2548,7 +3586,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3130,7 +4168,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3212,7 +4250,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-IN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3748,7 +4786,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4581,6 +5619,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -4588,7 +5627,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:gradFill flip="none" rotWithShape="1">
@@ -5417,6 +6455,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-4549-4415-9740-4578B96F6C0B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -5459,6 +6502,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-4549-4415-9740-4578B96F6C0B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -5501,6 +6549,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-4549-4415-9740-4578B96F6C0B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -5543,6 +6596,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-4549-4415-9740-4578B96F6C0B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -5585,6 +6643,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-4549-4415-9740-4578B96F6C0B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -6955,6 +8018,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -6962,7 +8026,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:gradFill flip="none" rotWithShape="1">
@@ -7329,6 +8392,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -7336,7 +8400,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:gradFill flip="none" rotWithShape="1">
@@ -7681,6 +8744,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -7688,7 +8752,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:gradFill flip="none" rotWithShape="1">
@@ -8015,6 +9078,86 @@
 </file>
 
 <file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10359,7 +11502,7 @@
 </file>
 
 <file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="257">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -10462,7 +11605,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -10472,7 +11615,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -10482,7 +11625,7 @@
     <cs:fillRef idx="3"/>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="34925" cap="rnd">
@@ -10502,7 +11645,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -10521,7 +11664,7 @@
     <cs:fillRef idx="3"/>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -10558,7 +11701,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -10582,7 +11725,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -10601,7 +11744,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -10619,7 +11762,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -10627,7 +11770,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -10646,7 +11789,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
@@ -10664,7 +11807,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -10683,7 +11826,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -10712,7 +11855,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -10720,7 +11863,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -10790,7 +11933,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
@@ -10816,7 +11959,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -10848,7 +11991,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -11847,6 +12990,998 @@
 </file>
 
 <file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -16766,6 +18901,83 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77EC2345-5F0F-5D3E-B0F8-3532D9493612}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DBDD7F6-6C17-9A82-5ED8-D696B5344757}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>443279</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -16839,7 +19051,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -17569,6 +19781,106 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19C594D1-B259-4952-973B-7C048043558D}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2018</v>
+      </c>
+      <c r="B2">
+        <v>265.60000000000002</v>
+      </c>
+      <c r="C2">
+        <v>237.1</v>
+      </c>
+      <c r="D2">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2019</v>
+      </c>
+      <c r="B3">
+        <v>260.10000000000002</v>
+      </c>
+      <c r="C3">
+        <v>232</v>
+      </c>
+      <c r="D3">
+        <v>28.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2020</v>
+      </c>
+      <c r="B4">
+        <v>274.5</v>
+      </c>
+      <c r="C4">
+        <v>244.2</v>
+      </c>
+      <c r="D4">
+        <v>30.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2021</v>
+      </c>
+      <c r="B5">
+        <v>365.8</v>
+      </c>
+      <c r="C5">
+        <v>310.5</v>
+      </c>
+      <c r="D5">
+        <v>55.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2022</v>
+      </c>
+      <c r="B6">
+        <v>385.9</v>
+      </c>
+      <c r="C6">
+        <v>334.7</v>
+      </c>
+      <c r="D6">
+        <v>51.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D0A681-0711-4BB4-8064-F007C13DFC22}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -17674,11 +19986,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2C59C6D-7FB4-4B0D-A95E-7AC709CADEF0}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
@@ -17781,12 +20093,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="46297aa2-77d1-4586-9726-07d56a535ee7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18019,20 +20333,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="46297aa2-77d1-4586-9726-07d56a535ee7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A006C7C1-35E5-4189-A4E2-5460DB68582D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E37863CE-6537-4A9C-A505-6059106A7573}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="631564f6-0349-4cc5-b00d-7cf3ba42f824"/>
+    <ds:schemaRef ds:uri="46297aa2-77d1-4586-9726-07d56a535ee7"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18057,12 +20372,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E37863CE-6537-4A9C-A505-6059106A7573}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A006C7C1-35E5-4189-A4E2-5460DB68582D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="631564f6-0349-4cc5-b00d-7cf3ba42f824"/>
-    <ds:schemaRef ds:uri="46297aa2-77d1-4586-9726-07d56a535ee7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>